<commit_message>
Commit after categorization using max and mean
</commit_message>
<xml_diff>
--- a/data/Stress Hyperglycemia Variable List.xlsx
+++ b/data/Stress Hyperglycemia Variable List.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C99AEF8A-E690-4E23-81B1-793F96EF8394}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8595838F-932A-4FB7-856F-536924D99A99}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="or_to_icu" sheetId="1" r:id="rId1"/>
@@ -2405,8 +2405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4720,8 +4720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07280A18-1BD1-4FDB-AB03-8EC8E7A45C01}">
   <dimension ref="A1:A158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4754,7 +4754,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>532</v>
       </c>

</xml_diff>

<commit_message>
Commit for initial CGM analysis plan
</commit_message>
<xml_diff>
--- a/data/Stress Hyperglycemia Variable List.xlsx
+++ b/data/Stress Hyperglycemia Variable List.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8595838F-932A-4FB7-856F-536924D99A99}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB99378-32C5-4CC8-91FF-F85EF9499F51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="or_to_icu" sheetId="1" r:id="rId1"/>
-    <sheet name="icu48h" sheetId="2" r:id="rId2"/>
-    <sheet name="cgm_summary" sheetId="3" r:id="rId3"/>
+    <sheet name="dt_surgery" sheetId="4" r:id="rId2"/>
+    <sheet name="icu48h" sheetId="2" r:id="rId3"/>
+    <sheet name="cgm_summary" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="690">
   <si>
     <t>variable</t>
   </si>
@@ -2077,6 +2078,21 @@
   </si>
   <si>
     <t>hbgi</t>
+  </si>
+  <si>
+    <t>Surgery start time</t>
+  </si>
+  <si>
+    <t>Surgery End Time</t>
+  </si>
+  <si>
+    <t>Length of surgery</t>
+  </si>
+  <si>
+    <t>surgery_start_time</t>
+  </si>
+  <si>
+    <t>surgery_end_time</t>
   </si>
 </sst>
 </file>
@@ -2405,8 +2421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3207,6 +3223,65 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FF6723E-FEDE-4F29-9272-6E8BFEC4F8C1}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="59.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>685</v>
+      </c>
+      <c r="B3" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>686</v>
+      </c>
+      <c r="B4" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>687</v>
+      </c>
+      <c r="B5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC267FE4-393C-41AC-8C1C-EE961F6FCDCC}">
   <dimension ref="A1:C184"/>
   <sheetViews>
@@ -4716,7 +4791,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07280A18-1BD1-4FDB-AB03-8EC8E7A45C01}">
   <dimension ref="A1:A158"/>
   <sheetViews>

</xml_diff>

<commit_message>
AHA Abstract + Code review pre-JL meeting
</commit_message>
<xml_diff>
--- a/data/Stress Hyperglycemia Variable List.xlsx
+++ b/data/Stress Hyperglycemia Variable List.xlsx
@@ -3,15 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB99378-32C5-4CC8-91FF-F85EF9499F51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA2925D-3E9B-408B-BAE0-0838B272CF2B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="or_to_icu" sheetId="1" r:id="rId1"/>
     <sheet name="dt_surgery" sheetId="4" r:id="rId2"/>
     <sheet name="icu48h" sheetId="2" r:id="rId3"/>
     <sheet name="cgm_summary" sheetId="3" r:id="rId4"/>
+    <sheet name="aha glucose" sheetId="5" r:id="rId5"/>
+    <sheet name="aha patient" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="887">
   <si>
     <t>variable</t>
   </si>
@@ -2093,6 +2095,597 @@
   </si>
   <si>
     <t>surgery_end_time</t>
+  </si>
+  <si>
+    <t>OR CGM value -Time 1</t>
+  </si>
+  <si>
+    <t>OR CGM Value1</t>
+  </si>
+  <si>
+    <t>OR CGM -Time2</t>
+  </si>
+  <si>
+    <t>OR CGM Value2</t>
+  </si>
+  <si>
+    <t>OR CGM -Time3</t>
+  </si>
+  <si>
+    <t>OR CGM Value3</t>
+  </si>
+  <si>
+    <t>OR CGM -Time 4</t>
+  </si>
+  <si>
+    <t>OR CGM Value 4</t>
+  </si>
+  <si>
+    <t>OR CGM -Time 5</t>
+  </si>
+  <si>
+    <t>OR CGM Value 5</t>
+  </si>
+  <si>
+    <t>OR CGM -Time 6</t>
+  </si>
+  <si>
+    <t>OR CGM Value 6</t>
+  </si>
+  <si>
+    <t>OR CGM -Time 7</t>
+  </si>
+  <si>
+    <t>OR CGM Value 7</t>
+  </si>
+  <si>
+    <t>OR CGM -Time 8</t>
+  </si>
+  <si>
+    <t>OR CGM Value 8</t>
+  </si>
+  <si>
+    <t>OR CGM -Time 9</t>
+  </si>
+  <si>
+    <t>OR CGM Value 9</t>
+  </si>
+  <si>
+    <t>OR CGM -Time 10</t>
+  </si>
+  <si>
+    <t>OR CGM Value 10</t>
+  </si>
+  <si>
+    <t>OR CGM -Time 11</t>
+  </si>
+  <si>
+    <t>OR CGM Value 11</t>
+  </si>
+  <si>
+    <t>OR CGM -Time 12</t>
+  </si>
+  <si>
+    <t>OR CGM Value 12</t>
+  </si>
+  <si>
+    <t>OR CGM -Time 13</t>
+  </si>
+  <si>
+    <t>OR CGM Value 13</t>
+  </si>
+  <si>
+    <t>OR CGM -Time 14</t>
+  </si>
+  <si>
+    <t>OR CGM Value 14</t>
+  </si>
+  <si>
+    <t>OR Time 15:</t>
+  </si>
+  <si>
+    <t>OR Time 16:</t>
+  </si>
+  <si>
+    <t>OR Time 17:</t>
+  </si>
+  <si>
+    <t>OR Time 18:</t>
+  </si>
+  <si>
+    <t>OR Time 19:</t>
+  </si>
+  <si>
+    <t>OR Time 20:</t>
+  </si>
+  <si>
+    <t>Number of BG values</t>
+  </si>
+  <si>
+    <t>Hyperglycemia BG &gt;180mg/dL</t>
+  </si>
+  <si>
+    <t>Hypoglycemia BG &lt; =70mg/dL and &gt;40mg/dL</t>
+  </si>
+  <si>
+    <t>Hypoglycemia BG &lt; =40mg/dL</t>
+  </si>
+  <si>
+    <t>Complete?</t>
+  </si>
+  <si>
+    <t>glucose_or15</t>
+  </si>
+  <si>
+    <t>time_or15</t>
+  </si>
+  <si>
+    <t>time_or17</t>
+  </si>
+  <si>
+    <t>time_or18</t>
+  </si>
+  <si>
+    <t>time_or19</t>
+  </si>
+  <si>
+    <t>time_or20</t>
+  </si>
+  <si>
+    <t>time_or16</t>
+  </si>
+  <si>
+    <t>glucose_or16</t>
+  </si>
+  <si>
+    <t>glucose_or17</t>
+  </si>
+  <si>
+    <t>glucose_or18</t>
+  </si>
+  <si>
+    <t>glucose_or19</t>
+  </si>
+  <si>
+    <t>glucose_or20</t>
+  </si>
+  <si>
+    <t>OR BG...8</t>
+  </si>
+  <si>
+    <t>OR BG...12</t>
+  </si>
+  <si>
+    <t>OR BG...16</t>
+  </si>
+  <si>
+    <t>OR BG...20</t>
+  </si>
+  <si>
+    <t>OR BG...24</t>
+  </si>
+  <si>
+    <t>OR BG...28</t>
+  </si>
+  <si>
+    <t>OR BG...32</t>
+  </si>
+  <si>
+    <t>OR BG...38</t>
+  </si>
+  <si>
+    <t>OR BG...40</t>
+  </si>
+  <si>
+    <t>OR BG...44</t>
+  </si>
+  <si>
+    <t>OR BG...48</t>
+  </si>
+  <si>
+    <t>OR BG...52</t>
+  </si>
+  <si>
+    <t>OR BG...56</t>
+  </si>
+  <si>
+    <t>OR BG...60</t>
+  </si>
+  <si>
+    <t>OR BG...64</t>
+  </si>
+  <si>
+    <t>OR BG...66</t>
+  </si>
+  <si>
+    <t>OR BG...68</t>
+  </si>
+  <si>
+    <t>OR BG...70</t>
+  </si>
+  <si>
+    <t>OR BG...72</t>
+  </si>
+  <si>
+    <t>OR BG...74</t>
+  </si>
+  <si>
+    <t>HyperglycemiaNumber of BG &gt;=140mg/dL</t>
+  </si>
+  <si>
+    <t>event_name</t>
+  </si>
+  <si>
+    <t>...2</t>
+  </si>
+  <si>
+    <t>HbA1c</t>
+  </si>
+  <si>
+    <t># of vessels</t>
+  </si>
+  <si>
+    <t>APACHE II</t>
+  </si>
+  <si>
+    <t>BMI</t>
+  </si>
+  <si>
+    <t>EF</t>
+  </si>
+  <si>
+    <t>pressor?</t>
+  </si>
+  <si>
+    <t>&gt;=2 pressors</t>
+  </si>
+  <si>
+    <t>AF</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Any cardiac complication? (MI, Arrhythmia, Cardiac arrest, Acute heart failure, vasopressors, inotropes)</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>Cardiac arrhythmia</t>
+  </si>
+  <si>
+    <t>Arrhythmias (choice=Frequent PVCs/PACs)</t>
+  </si>
+  <si>
+    <t>Arrhythmias (choice=VFib/Vtach)</t>
+  </si>
+  <si>
+    <t>Arrhythmias (choice=Cardiac arrest (Vfib/Vtach))</t>
+  </si>
+  <si>
+    <t>Arrhythmias (choice=Cardiac arrest (asystole, PEA))</t>
+  </si>
+  <si>
+    <t>Arrhythmias (choice=Other)</t>
+  </si>
+  <si>
+    <t>Specify (1):</t>
+  </si>
+  <si>
+    <t>Cardiac arrest</t>
+  </si>
+  <si>
+    <t>Pulmonary edema</t>
+  </si>
+  <si>
+    <t>Heart Failure</t>
+  </si>
+  <si>
+    <t>HTN</t>
+  </si>
+  <si>
+    <t>Hyperlipidemia</t>
+  </si>
+  <si>
+    <t>Alcohol</t>
+  </si>
+  <si>
+    <t>Smoking?</t>
+  </si>
+  <si>
+    <t>Never smoked</t>
+  </si>
+  <si>
+    <t>hba1c</t>
+  </si>
+  <si>
+    <t>ef</t>
+  </si>
+  <si>
+    <t>mi</t>
+  </si>
+  <si>
+    <t>hyperlipidemia</t>
+  </si>
+  <si>
+    <t>alcohol</t>
+  </si>
+  <si>
+    <t>n_vessels</t>
+  </si>
+  <si>
+    <t>apache_ii</t>
+  </si>
+  <si>
+    <t>pressor</t>
+  </si>
+  <si>
+    <t>ge2_pressor</t>
+  </si>
+  <si>
+    <t>cardiac_complication</t>
+  </si>
+  <si>
+    <t>cardiac_arrhythmia</t>
+  </si>
+  <si>
+    <t>cardiacarrest</t>
+  </si>
+  <si>
+    <t>hypertension</t>
+  </si>
+  <si>
+    <t>heartfailure</t>
+  </si>
+  <si>
+    <t>pulmonaryedema</t>
+  </si>
+  <si>
+    <t>smoking</t>
+  </si>
+  <si>
+    <t>neversmoked</t>
+  </si>
+  <si>
+    <t>arr_pvc</t>
+  </si>
+  <si>
+    <t>arr_vtach</t>
+  </si>
+  <si>
+    <t>arr_arrest_vfib</t>
+  </si>
+  <si>
+    <t>arr_arrest_asystolepea</t>
+  </si>
+  <si>
+    <t>arr_other</t>
+  </si>
+  <si>
+    <t>afib</t>
+  </si>
+  <si>
+    <t>BG...84</t>
+  </si>
+  <si>
+    <t>BG...86</t>
+  </si>
+  <si>
+    <t>BG...88</t>
+  </si>
+  <si>
+    <t>BG...90</t>
+  </si>
+  <si>
+    <t>BG...92</t>
+  </si>
+  <si>
+    <t>BG...94</t>
+  </si>
+  <si>
+    <t>BG...96</t>
+  </si>
+  <si>
+    <t>BG...98</t>
+  </si>
+  <si>
+    <t>BG...100</t>
+  </si>
+  <si>
+    <t>BG...102</t>
+  </si>
+  <si>
+    <t>BG...104</t>
+  </si>
+  <si>
+    <t>BG...106</t>
+  </si>
+  <si>
+    <t>BG...108</t>
+  </si>
+  <si>
+    <t>BG...110</t>
+  </si>
+  <si>
+    <t>BG...112</t>
+  </si>
+  <si>
+    <t>BG...114</t>
+  </si>
+  <si>
+    <t>Time 17:</t>
+  </si>
+  <si>
+    <t>BG...116</t>
+  </si>
+  <si>
+    <t>Time 18:</t>
+  </si>
+  <si>
+    <t>BG...118</t>
+  </si>
+  <si>
+    <t>Time 19:</t>
+  </si>
+  <si>
+    <t>BG...120</t>
+  </si>
+  <si>
+    <t>Time 20:</t>
+  </si>
+  <si>
+    <t>BG...122</t>
+  </si>
+  <si>
+    <t>Time 21:</t>
+  </si>
+  <si>
+    <t>BG...124</t>
+  </si>
+  <si>
+    <t>Time 22:</t>
+  </si>
+  <si>
+    <t>BG...126</t>
+  </si>
+  <si>
+    <t>Time 23:</t>
+  </si>
+  <si>
+    <t>BG...128</t>
+  </si>
+  <si>
+    <t>Time 24:</t>
+  </si>
+  <si>
+    <t>BG...130</t>
+  </si>
+  <si>
+    <t>Time 25:</t>
+  </si>
+  <si>
+    <t>BG...132</t>
+  </si>
+  <si>
+    <t>Time 26:</t>
+  </si>
+  <si>
+    <t>BG...134</t>
+  </si>
+  <si>
+    <t>Time 27:</t>
+  </si>
+  <si>
+    <t>BG...136</t>
+  </si>
+  <si>
+    <t>Time 28:</t>
+  </si>
+  <si>
+    <t>BG...138</t>
+  </si>
+  <si>
+    <t>Time 29:</t>
+  </si>
+  <si>
+    <t>BG...140</t>
+  </si>
+  <si>
+    <t>Time 30:</t>
+  </si>
+  <si>
+    <t>BG...142</t>
+  </si>
+  <si>
+    <t>HyperglycemiaNumber of BF &gt;140mg/dL</t>
+  </si>
+  <si>
+    <t>Hyperglycemia BG &gt; 180mg/dL:</t>
+  </si>
+  <si>
+    <t>time_icu17</t>
+  </si>
+  <si>
+    <t>glucose_icu17</t>
+  </si>
+  <si>
+    <t>time_icu18</t>
+  </si>
+  <si>
+    <t>glucose_icu18</t>
+  </si>
+  <si>
+    <t>time_icu19</t>
+  </si>
+  <si>
+    <t>glucose_icu19</t>
+  </si>
+  <si>
+    <t>time_icu20</t>
+  </si>
+  <si>
+    <t>glucose_icu20</t>
+  </si>
+  <si>
+    <t>time_icu21</t>
+  </si>
+  <si>
+    <t>glucose_icu21</t>
+  </si>
+  <si>
+    <t>time_icu22</t>
+  </si>
+  <si>
+    <t>glucose_icu22</t>
+  </si>
+  <si>
+    <t>time_icu23</t>
+  </si>
+  <si>
+    <t>glucose_icu23</t>
+  </si>
+  <si>
+    <t>time_icu24</t>
+  </si>
+  <si>
+    <t>glucose_icu24</t>
+  </si>
+  <si>
+    <t>time_icu25</t>
+  </si>
+  <si>
+    <t>glucose_icu25</t>
+  </si>
+  <si>
+    <t>time_icu26</t>
+  </si>
+  <si>
+    <t>glucose_icu26</t>
+  </si>
+  <si>
+    <t>time_icu27</t>
+  </si>
+  <si>
+    <t>glucose_icu27</t>
+  </si>
+  <si>
+    <t>time_icu28</t>
+  </si>
+  <si>
+    <t>glucose_icu28</t>
+  </si>
+  <si>
+    <t>time_icu29</t>
+  </si>
+  <si>
+    <t>glucose_icu29</t>
+  </si>
+  <si>
+    <t>time_icu30</t>
+  </si>
+  <si>
+    <t>glucose_icu30</t>
   </si>
 </sst>
 </file>
@@ -2421,8 +3014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3226,8 +3819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FF6723E-FEDE-4F29-9272-6E8BFEC4F8C1}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3285,8 +3878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC267FE4-393C-41AC-8C1C-EE961F6FCDCC}">
   <dimension ref="A1:C184"/>
   <sheetViews>
-    <sheetView topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="A145" sqref="A145"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5597,4 +6190,1345 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F730E738-71E8-4BB9-9BDD-FAFBA3CE3EC3}">
+  <dimension ref="A1:B146"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="56.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>687</v>
+      </c>
+      <c r="B4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>685</v>
+      </c>
+      <c r="B5" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>686</v>
+      </c>
+      <c r="B6" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>741</v>
+      </c>
+      <c r="B9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>742</v>
+      </c>
+      <c r="B13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>743</v>
+      </c>
+      <c r="B17" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>744</v>
+      </c>
+      <c r="B21" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>745</v>
+      </c>
+      <c r="B25" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>746</v>
+      </c>
+      <c r="B29" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>747</v>
+      </c>
+      <c r="B33" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>748</v>
+      </c>
+      <c r="B39" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>749</v>
+      </c>
+      <c r="B41" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>28</v>
+      </c>
+      <c r="B44" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>750</v>
+      </c>
+      <c r="B45" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>30</v>
+      </c>
+      <c r="B48" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>751</v>
+      </c>
+      <c r="B49" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>32</v>
+      </c>
+      <c r="B52" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>752</v>
+      </c>
+      <c r="B53" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>34</v>
+      </c>
+      <c r="B56" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>753</v>
+      </c>
+      <c r="B57" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>36</v>
+      </c>
+      <c r="B60" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>754</v>
+      </c>
+      <c r="B61" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>718</v>
+      </c>
+      <c r="B64" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>755</v>
+      </c>
+      <c r="B65" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>719</v>
+      </c>
+      <c r="B66" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>756</v>
+      </c>
+      <c r="B67" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>720</v>
+      </c>
+      <c r="B68" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>757</v>
+      </c>
+      <c r="B69" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>721</v>
+      </c>
+      <c r="B70" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>758</v>
+      </c>
+      <c r="B71" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>722</v>
+      </c>
+      <c r="B72" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>759</v>
+      </c>
+      <c r="B73" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>723</v>
+      </c>
+      <c r="B74" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>760</v>
+      </c>
+      <c r="B75" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>8</v>
+      </c>
+      <c r="B83" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>193</v>
+      </c>
+      <c r="B84" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>813</v>
+      </c>
+      <c r="B85" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>194</v>
+      </c>
+      <c r="B86" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>814</v>
+      </c>
+      <c r="B87" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>195</v>
+      </c>
+      <c r="B88" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>815</v>
+      </c>
+      <c r="B89" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>196</v>
+      </c>
+      <c r="B90" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>816</v>
+      </c>
+      <c r="B91" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>198</v>
+      </c>
+      <c r="B92" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>817</v>
+      </c>
+      <c r="B93" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>200</v>
+      </c>
+      <c r="B94" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>818</v>
+      </c>
+      <c r="B95" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>202</v>
+      </c>
+      <c r="B96" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>819</v>
+      </c>
+      <c r="B97" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>204</v>
+      </c>
+      <c r="B98" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>820</v>
+      </c>
+      <c r="B99" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>206</v>
+      </c>
+      <c r="B100" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>821</v>
+      </c>
+      <c r="B101" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>208</v>
+      </c>
+      <c r="B102" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>822</v>
+      </c>
+      <c r="B103" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>210</v>
+      </c>
+      <c r="B104" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>823</v>
+      </c>
+      <c r="B105" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>212</v>
+      </c>
+      <c r="B106" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>824</v>
+      </c>
+      <c r="B107" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>214</v>
+      </c>
+      <c r="B108" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>825</v>
+      </c>
+      <c r="B109" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>216</v>
+      </c>
+      <c r="B110" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>826</v>
+      </c>
+      <c r="B111" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>218</v>
+      </c>
+      <c r="B112" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>827</v>
+      </c>
+      <c r="B113" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>220</v>
+      </c>
+      <c r="B114" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>828</v>
+      </c>
+      <c r="B115" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>829</v>
+      </c>
+      <c r="B116" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>830</v>
+      </c>
+      <c r="B117" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>831</v>
+      </c>
+      <c r="B118" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>832</v>
+      </c>
+      <c r="B119" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>833</v>
+      </c>
+      <c r="B120" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>834</v>
+      </c>
+      <c r="B121" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>835</v>
+      </c>
+      <c r="B122" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>836</v>
+      </c>
+      <c r="B123" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>837</v>
+      </c>
+      <c r="B124" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>838</v>
+      </c>
+      <c r="B125" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>839</v>
+      </c>
+      <c r="B126" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>840</v>
+      </c>
+      <c r="B127" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>841</v>
+      </c>
+      <c r="B128" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>842</v>
+      </c>
+      <c r="B129" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>843</v>
+      </c>
+      <c r="B130" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>844</v>
+      </c>
+      <c r="B131" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>845</v>
+      </c>
+      <c r="B132" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>846</v>
+      </c>
+      <c r="B133" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>847</v>
+      </c>
+      <c r="B134" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>848</v>
+      </c>
+      <c r="B135" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>849</v>
+      </c>
+      <c r="B136" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>850</v>
+      </c>
+      <c r="B137" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>851</v>
+      </c>
+      <c r="B138" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>852</v>
+      </c>
+      <c r="B139" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>853</v>
+      </c>
+      <c r="B140" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>854</v>
+      </c>
+      <c r="B141" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>855</v>
+      </c>
+      <c r="B142" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>856</v>
+      </c>
+      <c r="B143" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>858</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A7ED6AA-780D-40B6-8131-5D17C4E940B1}">
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="90.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>764</v>
+      </c>
+      <c r="B4" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>687</v>
+      </c>
+      <c r="B5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>765</v>
+      </c>
+      <c r="B6" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>766</v>
+      </c>
+      <c r="B7" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>513</v>
+      </c>
+      <c r="B8" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>511</v>
+      </c>
+      <c r="B9" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>767</v>
+      </c>
+      <c r="B10" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>768</v>
+      </c>
+      <c r="B11" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>769</v>
+      </c>
+      <c r="B12" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>770</v>
+      </c>
+      <c r="B13" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>771</v>
+      </c>
+      <c r="B14" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>772</v>
+      </c>
+      <c r="B15" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>773</v>
+      </c>
+      <c r="B16" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>774</v>
+      </c>
+      <c r="B17" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>775</v>
+      </c>
+      <c r="B18" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>776</v>
+      </c>
+      <c r="B19" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>777</v>
+      </c>
+      <c r="B20" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>778</v>
+      </c>
+      <c r="B21" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>779</v>
+      </c>
+      <c r="B22" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>780</v>
+      </c>
+      <c r="B23" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>782</v>
+      </c>
+      <c r="B25" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>783</v>
+      </c>
+      <c r="B26" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>784</v>
+      </c>
+      <c r="B27" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>785</v>
+      </c>
+      <c r="B28" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>786</v>
+      </c>
+      <c r="B29" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>787</v>
+      </c>
+      <c r="B30" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>788</v>
+      </c>
+      <c r="B31" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>789</v>
+      </c>
+      <c r="B32" t="s">
+        <v>806</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>